<commit_message>
week 11 reading and inputs
</commit_message>
<xml_diff>
--- a/observations/Observations.xlsx
+++ b/observations/Observations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nareshpanta/Documents/GitHub/imperial-ai-ml-capstone-project/observations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3261A7C-955B-9144-B31F-C9407AD8F8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640A3CDB-3EE5-1E4F-B077-143D7666361A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17540" xr2:uid="{879C9F3D-DEC7-554E-8B9E-2E328A028C98}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17540" activeTab="11" xr2:uid="{879C9F3D-DEC7-554E-8B9E-2E328A028C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Week8" sheetId="10" r:id="rId9"/>
     <sheet name="Week9" sheetId="11" r:id="rId10"/>
     <sheet name="Week10" sheetId="12" r:id="rId11"/>
+    <sheet name="Week11" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="204">
   <si>
     <t>Function</t>
   </si>
@@ -626,6 +627,42 @@
   </si>
   <si>
     <t>0.474747-0.444444-0.363636</t>
+  </si>
+  <si>
+    <t>GP and EI. Changed EI to 0.001 from 0.01 for exploitation</t>
+  </si>
+  <si>
+    <t>0.787879-0.919192</t>
+  </si>
+  <si>
+    <t>GP and changed from UCB to EI with xi=0.01</t>
+  </si>
+  <si>
+    <t>0.401976-0.362499-0.443216-0.362051</t>
+  </si>
+  <si>
+    <t>GP and UCB with kappa=1</t>
+  </si>
+  <si>
+    <t>0.405247-0.994863-0.998796-0.997793</t>
+  </si>
+  <si>
+    <t>SVM. Changed C back to 1 from 5</t>
+  </si>
+  <si>
+    <t>0.423065-0.335611-0.549974-0.769547-0.114872</t>
+  </si>
+  <si>
+    <t>SVM continiue with C=5</t>
+  </si>
+  <si>
+    <t>0.001165-0.304194-0.258543-0.284629-0.258669-0.614834</t>
+  </si>
+  <si>
+    <t>SVM with C=10</t>
+  </si>
+  <si>
+    <t>0.097805-0.249076-0.092150-0.283382-0.631658-0.456355-0.291001-0.613192</t>
   </si>
 </sst>
 </file>
@@ -745,12 +782,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F054F69-D94D-D64A-81C5-4411182D0207}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44:L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1101,25 +1138,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -1659,19 +1696,23 @@
         <f>Week9!F2</f>
         <v>5.2647530338544495E-57</v>
       </c>
+      <c r="K27" s="3">
+        <f>Week10!F2</f>
+        <v>1.7063022014990999E-17</v>
+      </c>
       <c r="P27" s="3" t="str">
         <f>INDEX($B$26:$M$26, MATCH(MAX(B27:M27), B27:M27, 0))</f>
-        <v>Week8</v>
+        <v>Week10</v>
       </c>
       <c r="Q27" s="3">
         <f>MAX(B27:M27)</f>
-        <v>1.55842898547174E-23</v>
-      </c>
-      <c r="R27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="34">
+        <v>1.7063022014990999E-17</v>
+      </c>
+      <c r="R27" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="17">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1711,16 +1752,20 @@
         <f>Week9!F3</f>
         <v>0.63564435544545905</v>
       </c>
+      <c r="K28" s="3">
+        <f>Week10!F3</f>
+        <v>0.72074952220389799</v>
+      </c>
       <c r="P28" s="3" t="str">
         <f t="shared" ref="P28:P34" si="0">INDEX($B$26:$M$26, MATCH(MAX(B28:M28), B28:M28, 0))</f>
-        <v>Week9</v>
+        <v>Week10</v>
       </c>
       <c r="Q28" s="3">
         <f t="shared" ref="Q28:Q34" si="1">MAX(B28:M28)</f>
-        <v>0.63564435544545905</v>
+        <v>0.72074952220389799</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="17">
@@ -1763,6 +1808,10 @@
         <f>Week9!F4</f>
         <v>-2.6296009521582001E-3</v>
       </c>
+      <c r="K29" s="3">
+        <f>Week10!F4</f>
+        <v>-2.8096226155954401E-2</v>
+      </c>
       <c r="P29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Week9</v>
@@ -1772,7 +1821,7 @@
         <v>-2.6296009521582001E-3</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1815,6 +1864,10 @@
         <f>Week9!F5</f>
         <v>0.57701270290822404</v>
       </c>
+      <c r="K30" s="3">
+        <f>Week10!F5</f>
+        <v>-1.0498889373006599</v>
+      </c>
       <c r="P30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Week7</v>
@@ -1867,13 +1920,17 @@
         <f>Week9!F6</f>
         <v>4189.1605631845196</v>
       </c>
+      <c r="K31" s="3">
+        <f>Week10!F6</f>
+        <v>4537.8399923503803</v>
+      </c>
       <c r="P31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Week7</v>
+        <v>Week10</v>
       </c>
       <c r="Q31" s="3">
         <f t="shared" si="1"/>
-        <v>4310.9805594415402</v>
+        <v>4537.8399923503803</v>
       </c>
       <c r="R31" t="s">
         <v>78</v>
@@ -1919,6 +1976,10 @@
         <f>Week9!F7</f>
         <v>-0.14749973636875199</v>
       </c>
+      <c r="K32" s="3">
+        <f>Week10!F7</f>
+        <v>-0.222075655316051</v>
+      </c>
       <c r="P32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Week4</v>
@@ -1971,13 +2032,17 @@
         <f>Week9!F8</f>
         <v>1.7512570814124699</v>
       </c>
+      <c r="K33" s="3">
+        <f>Week10!F8</f>
+        <v>1.92969449721477</v>
+      </c>
       <c r="P33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Week6</v>
+        <v>Week10</v>
       </c>
       <c r="Q33" s="3">
         <f t="shared" si="1"/>
-        <v>1.88380795677045</v>
+        <v>1.92969449721477</v>
       </c>
       <c r="R33" t="s">
         <v>79</v>
@@ -2023,6 +2088,10 @@
         <f>Week9!F9</f>
         <v>6.4336900000000004</v>
       </c>
+      <c r="K34" s="3">
+        <f>Week10!F9</f>
+        <v>9.9444201092011006</v>
+      </c>
       <c r="P34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Week6</v>
@@ -2115,6 +2184,9 @@
       <c r="K39" s="14" t="s">
         <v>188</v>
       </c>
+      <c r="L39" s="13" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="40" spans="1:18" ht="21" customHeight="1">
       <c r="A40">
@@ -2150,6 +2222,9 @@
       <c r="K40" s="13" t="s">
         <v>188</v>
       </c>
+      <c r="L40" s="13" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="41" spans="1:18" ht="23" customHeight="1">
       <c r="A41">
@@ -2185,6 +2260,9 @@
       <c r="K41" s="13" t="s">
         <v>188</v>
       </c>
+      <c r="L41" s="13" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="42" spans="1:18" ht="19" customHeight="1">
       <c r="A42">
@@ -2220,6 +2298,9 @@
       <c r="K42" s="14" t="s">
         <v>78</v>
       </c>
+      <c r="L42" s="13" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="43" spans="1:18" s="14" customFormat="1" ht="23" customHeight="1">
       <c r="A43" s="14">
@@ -2255,8 +2336,11 @@
       <c r="K43" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" ht="34">
+      <c r="L43" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="17">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2288,6 +2372,9 @@
         <v>177</v>
       </c>
       <c r="K44" t="s">
+        <v>79</v>
+      </c>
+      <c r="L44" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2325,6 +2412,9 @@
       <c r="K45" t="s">
         <v>79</v>
       </c>
+      <c r="L45" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="46" spans="1:18" ht="17">
       <c r="A46">
@@ -2358,6 +2448,9 @@
         <v>179</v>
       </c>
       <c r="K46" t="s">
+        <v>79</v>
+      </c>
+      <c r="L46" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2429,7 +2522,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>171</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -2465,7 +2558,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>172</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -2500,7 +2593,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>173</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -2535,7 +2628,7 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>174</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -2570,7 +2663,7 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>175</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -2605,7 +2698,7 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>176</v>
       </c>
       <c r="D7" s="13" t="s">
@@ -2640,7 +2733,7 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>178</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -3155,7 +3248,822 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9F4F33-0F72-E045-9A1C-A86F31202424}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" s="11">
+        <v>7.7108751145028402E-16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1.7063022014990999E-17</v>
+      </c>
+      <c r="G2" s="8">
+        <f>(ABS(E2 -F2)/MAX(ABS(E2),ABS(F2)) )* 100</f>
+        <v>97.787148441439754</v>
+      </c>
+      <c r="H2" s="8">
+        <f xml:space="preserve"> Week4!G2 - Week10!G2</f>
+        <v>2.2128515585602457</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="12">
+        <v>-1.82610597959317E-4</v>
+      </c>
+      <c r="K2">
+        <f>ABS(F2) - ABS(J2)</f>
+        <v>-1.8261059795929993E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0.63564435544545905</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.72074952220389799</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G9" si="0">(ABS(E3 -F3)/MAX(ABS(E3),ABS(F3)) )* 100</f>
+        <v>11.807870020947849</v>
+      </c>
+      <c r="H3" s="8">
+        <f xml:space="preserve"> Week4!G3 - Week10!G3</f>
+        <v>5.1900150842701791</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0.680331821170302</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K9" si="1">ABS(F3) - ABS(J3)</f>
+        <v>4.0417701033595987E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="12">
+        <v>-2.6296009521582001E-3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>-2.8096226155954401E-2</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>90.640732539800865</v>
+      </c>
+      <c r="H4" s="8">
+        <f xml:space="preserve"> Week4!G4 - Week10!G4</f>
+        <v>-34.316054971512727</v>
+      </c>
+      <c r="J4" s="12">
+        <v>-1.53417251817563E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>1.2754500974198101E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.57749759425457003</v>
+      </c>
+      <c r="F5" s="5">
+        <v>-1.0498889373006599</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
+        <v>155.00558904252847</v>
+      </c>
+      <c r="H5" s="8">
+        <f xml:space="preserve"> Week4!G5 - Week10!G5</f>
+        <v>-75.163482888473581</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.52942733383851404</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0.52046160346214587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="12">
+        <v>4310.9805594415402</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4537.8399923503803</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>4.9992823301673521</v>
+      </c>
+      <c r="H6" s="8">
+        <f xml:space="preserve"> Week4!G6 - Week10!G6</f>
+        <v>33.496637213798927</v>
+      </c>
+      <c r="J6" s="12">
+        <v>3773.9891608299399</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>763.85083152044035</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="12">
+        <v>-0.12430862230397099</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-0.222075655316051</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>44.024201064696207</v>
+      </c>
+      <c r="H7" s="8">
+        <f xml:space="preserve"> Week4!G7 - Week10!G7</f>
+        <v>17.705513263185914</v>
+      </c>
+      <c r="J7" s="12">
+        <v>-0.22564673102918401</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>-3.571075713133004E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1.88380795677045</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1.92969449721477</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.3779173600044214</v>
+      </c>
+      <c r="H8" s="8">
+        <f xml:space="preserve"> Week4!G8 - Week10!G8</f>
+        <v>36.003341592721242</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1.79243618860138</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.13725830861339006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="12">
+        <v>9.9707717627203998</v>
+      </c>
+      <c r="F9" s="5">
+        <v>9.9444201092011006</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.26428900536892258</v>
+      </c>
+      <c r="H9" s="8">
+        <f xml:space="preserve"> Week4!G9 - Week10!G9</f>
+        <v>-0.19138452857587152</v>
+      </c>
+      <c r="J9" s="12">
+        <v>10.051246412332</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>-0.1068263031308998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="11">
+        <v>7.7108751145028402E-16</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="8" t="e">
+        <f>(ABS(#REF! -F14)/MAX(ABS(#REF!),ABS(F14)) )* 100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H14" s="8" t="e">
+        <f xml:space="preserve"> Week3!G14 - Week10!G14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="12">
+        <v>-1.82610597959317E-4</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="18">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0.63564435544545905</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="8">
+        <f t="shared" ref="G15:G21" si="2">(ABS(E15 -F15)/MAX(ABS(E15),ABS(F15)) )* 100</f>
+        <v>100</v>
+      </c>
+      <c r="H15" s="8">
+        <f xml:space="preserve"> Week3!G15 - Week10!G15</f>
+        <v>-100</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0.680331821170302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="18">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="12">
+        <v>-2.6296009521582001E-3</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H16" s="8">
+        <f xml:space="preserve"> Week3!G16 - Week10!G16</f>
+        <v>-100</v>
+      </c>
+      <c r="J16" s="12">
+        <v>-1.53417251817563E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.57749759425457003</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="8">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H17" s="8">
+        <f xml:space="preserve"> Week3!G17 - Week10!G17</f>
+        <v>-100</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.52942733383851404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="12">
+        <v>4310.9805594415402</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="8">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H18" s="8">
+        <f xml:space="preserve"> Week3!G18 - Week10!G18</f>
+        <v>-100</v>
+      </c>
+      <c r="J18" s="12">
+        <v>3773.9891608299399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="8" t="e">
+        <f xml:space="preserve"> Week3!G19 - Week10!G19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" ht="18">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="8" t="e">
+        <f xml:space="preserve"> Week3!G20 - Week10!G20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" ht="18">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="8" t="e">
+        <f xml:space="preserve"> Week3!G21 - Week10!G21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="18">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="8" t="e">
+        <f>(ABS(E28 -F28)/MAX(ABS(E28),ABS(F28)) )* 100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="8" t="e">
+        <f xml:space="preserve"> Week3!G2 - Week10!G28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:12" ht="18">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="8" t="e">
+        <f t="shared" ref="G29:G35" si="3">(ABS(E29 -F29)/MAX(ABS(E29),ABS(F29)) )* 100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="8" t="e">
+        <f xml:space="preserve"> Week3!G3 - Week10!G29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" ht="18">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="12"/>
+      <c r="G30" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="8" t="e">
+        <f xml:space="preserve"> Week3!G4 - Week10!G30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:12" ht="18">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="8" t="e">
+        <f xml:space="preserve"> Week3!G5 - Week10!G31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:12" ht="18">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="8" t="e">
+        <f xml:space="preserve"> Week3!G6 - Week10!G32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" ht="18">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="12">
+        <v>-0.12430862230397099</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H33" s="8">
+        <f xml:space="preserve"> Week3!G7 - Week10!G33</f>
+        <v>-38.753477525597134</v>
+      </c>
+      <c r="J33" s="12">
+        <v>-0.22564673102918401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="18">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="12">
+        <v>1.88380795677045</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H34" s="8">
+        <f xml:space="preserve"> Week3!G8 - Week10!G34</f>
+        <v>-70.691643968564648</v>
+      </c>
+      <c r="J34" s="12">
+        <v>1.79243618860138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="18">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="12">
+        <v>9.9707717627203998</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H35" s="8">
+        <f xml:space="preserve"> Week3!G9 - Week10!G35</f>
+        <v>-97.559723769512345</v>
+      </c>
+      <c r="J35" s="12">
+        <v>10.051246412332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0A6397-1792-FC49-8FB0-C74C348251FE}">
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3204,7 +4112,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18">
+    <row r="2" spans="1:11" ht="34">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3212,10 +4120,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E2" s="11">
         <v>7.7108751145028402E-16</v>
@@ -3226,19 +4134,15 @@
         <v>100</v>
       </c>
       <c r="H2" s="8">
-        <f xml:space="preserve"> Week4!G2 - Week10!G2</f>
+        <f xml:space="preserve"> Week4!G2 - Week11!G2</f>
         <v>0</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="12">
-        <v>-1.82610597959317E-4</v>
-      </c>
-      <c r="K2">
-        <f>ABS(F2) - ABS(J2)</f>
-        <v>-1.82610597959317E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18">
+        <v>-1.4302305791296299E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="34">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3249,10 +4153,10 @@
         <v>190</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E3" s="12">
-        <v>0.63564435544545905</v>
+        <v>0.72074952220389799</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="8">
@@ -3260,18 +4164,14 @@
         <v>100</v>
       </c>
       <c r="H3" s="8">
-        <f xml:space="preserve"> Week4!G3 - Week10!G3</f>
+        <f xml:space="preserve"> Week4!G3 - Week11!G3</f>
         <v>-83.002114894781968</v>
       </c>
       <c r="J3" s="12">
         <v>0.680331821170302</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K9" si="1">ABS(F3) - ABS(J3)</f>
-        <v>-0.680331821170302</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18">
+    </row>
+    <row r="4" spans="1:11" ht="34">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3282,7 +4182,7 @@
         <v>191</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E4" s="12">
         <v>-2.6296009521582001E-3</v>
@@ -3293,18 +4193,14 @@
         <v>100</v>
       </c>
       <c r="H4" s="8">
-        <f xml:space="preserve"> Week4!G4 - Week10!G4</f>
+        <f xml:space="preserve"> Week4!G4 - Week11!G4</f>
         <v>-43.675322431711862</v>
       </c>
       <c r="J4" s="12">
         <v>-1.53417251817563E-2</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>-1.53417251817563E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="18">
+    </row>
+    <row r="5" spans="1:11" ht="34">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3312,10 +4208,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="E5" s="12">
         <v>0.57749759425457003</v>
@@ -3326,15 +4222,11 @@
         <v>100</v>
       </c>
       <c r="H5" s="8">
-        <f xml:space="preserve"> Week4!G5 - Week10!G5</f>
+        <f xml:space="preserve"> Week4!G5 - Week11!G5</f>
         <v>-20.157893845945111</v>
       </c>
       <c r="J5" s="12">
-        <v>0.52942733383851404</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>-0.52942733383851404</v>
+        <v>1.03862596115182</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="18">
@@ -3345,13 +4237,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E6" s="12">
-        <v>4310.9805594415402</v>
+        <v>4537.8399923503803</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="8">
@@ -3359,15 +4251,11 @@
         <v>100</v>
       </c>
       <c r="H6" s="8">
-        <f xml:space="preserve"> Week4!G6 - Week10!G6</f>
+        <f xml:space="preserve"> Week4!G6 - Week11!G6</f>
         <v>-61.504080456033719</v>
       </c>
       <c r="J6" s="12">
-        <v>3773.9891608299399</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>-3773.9891608299399</v>
+        <v>4531.9910287256898</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="18">
@@ -3378,10 +4266,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="E7" s="12">
         <v>-0.12430862230397099</v>
@@ -3392,15 +4280,11 @@
         <v>100</v>
       </c>
       <c r="H7" s="8">
-        <f xml:space="preserve"> Week4!G7 - Week10!G7</f>
+        <f xml:space="preserve"> Week4!G7 - Week11!G7</f>
         <v>-38.270285672117879</v>
       </c>
       <c r="J7" s="12">
-        <v>-0.22564673102918401</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>-0.22564673102918401</v>
+        <v>-0.24925084580634199</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18">
@@ -3411,13 +4295,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="E8" s="12">
-        <v>1.88380795677045</v>
+        <v>1.92969449721477</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="8">
@@ -3425,15 +4309,11 @@
         <v>100</v>
       </c>
       <c r="H8" s="8">
-        <f xml:space="preserve"> Week4!G8 - Week10!G8</f>
+        <f xml:space="preserve"> Week4!G8 - Week11!G8</f>
         <v>-61.618741047274334</v>
       </c>
       <c r="J8" s="12">
-        <v>1.79243618860138</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>-1.79243618860138</v>
+        <v>1.82254519575486</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="18">
@@ -3444,10 +4324,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="E9" s="12">
         <v>9.9707717627203998</v>
@@ -3458,15 +4338,11 @@
         <v>100</v>
       </c>
       <c r="H9" s="8">
-        <f xml:space="preserve"> Week4!G9 - Week10!G9</f>
+        <f xml:space="preserve"> Week4!G9 - Week11!G9</f>
         <v>-99.927095523206944</v>
       </c>
       <c r="J9" s="12">
-        <v>10.051246412332</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>-10.051246412332</v>
+        <v>10.0604203159638</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -3506,7 +4382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18">
+    <row r="14" spans="1:11" ht="34">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3514,10 +4390,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E14" s="11">
         <v>7.7108751145028402E-16</v>
@@ -3528,15 +4404,15 @@
         <v>#REF!</v>
       </c>
       <c r="H14" s="8" t="e">
-        <f xml:space="preserve"> Week3!G14 - Week10!G14</f>
+        <f xml:space="preserve"> Week3!G14 - Week11!G14</f>
         <v>#REF!</v>
       </c>
       <c r="J14" s="12">
-        <v>-1.82610597959317E-4</v>
+        <v>-1.4302305791296299E-4</v>
       </c>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="18">
+    <row r="15" spans="1:11" ht="34">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3547,25 +4423,25 @@
         <v>190</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E15" s="12">
-        <v>0.63564435544545905</v>
+        <v>0.72074952220389799</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="8">
-        <f t="shared" ref="G15:G21" si="2">(ABS(E15 -F15)/MAX(ABS(E15),ABS(F15)) )* 100</f>
+        <f t="shared" ref="G15:G21" si="1">(ABS(E15 -F15)/MAX(ABS(E15),ABS(F15)) )* 100</f>
         <v>100</v>
       </c>
       <c r="H15" s="8">
-        <f xml:space="preserve"> Week3!G15 - Week10!G15</f>
+        <f xml:space="preserve"> Week3!G15 - Week11!G15</f>
         <v>-100</v>
       </c>
       <c r="J15" s="12">
         <v>0.680331821170302</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18">
+    <row r="16" spans="1:11" ht="34">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3576,24 +4452,24 @@
         <v>191</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E16" s="12">
         <v>-2.6296009521582001E-3</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H16" s="8">
-        <f xml:space="preserve"> Week3!G16 - Week10!G16</f>
+        <f xml:space="preserve"> Week3!G16 - Week11!G16</f>
         <v>-100</v>
       </c>
       <c r="J16" s="12">
         <v>-1.53417251817563E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18">
+    <row r="17" spans="1:12" ht="34">
       <c r="A17">
         <v>4</v>
       </c>
@@ -3601,25 +4477,25 @@
         <v>4</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="E17" s="12">
         <v>0.57749759425457003</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H17" s="8">
-        <f xml:space="preserve"> Week3!G17 - Week10!G17</f>
+        <f xml:space="preserve"> Week3!G17 - Week11!G17</f>
         <v>-100</v>
       </c>
       <c r="J17" s="12">
-        <v>0.52942733383851404</v>
+        <v>1.03862596115182</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18">
@@ -3630,25 +4506,25 @@
         <v>5</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E18" s="12">
-        <v>4310.9805594415402</v>
+        <v>4537.8399923503803</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H18" s="8">
-        <f xml:space="preserve"> Week3!G18 - Week10!G18</f>
+        <f xml:space="preserve"> Week3!G18 - Week11!G18</f>
         <v>-100</v>
       </c>
       <c r="J18" s="12">
-        <v>3773.9891608299399</v>
+        <v>4531.9910287256898</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18">
@@ -3663,11 +4539,11 @@
       <c r="E19" s="12"/>
       <c r="F19" s="5"/>
       <c r="G19" s="8" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H19" s="8" t="e">
-        <f xml:space="preserve"> Week3!G19 - Week10!G19</f>
+        <f xml:space="preserve"> Week3!G19 - Week11!G19</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J19" s="12"/>
@@ -3684,11 +4560,11 @@
       <c r="E20" s="12"/>
       <c r="F20" s="5"/>
       <c r="G20" s="8" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H20" s="8" t="e">
-        <f xml:space="preserve"> Week3!G20 - Week10!G20</f>
+        <f xml:space="preserve"> Week3!G20 - Week11!G20</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J20" s="12"/>
@@ -3705,11 +4581,11 @@
       <c r="E21" s="12"/>
       <c r="F21" s="5"/>
       <c r="G21" s="8" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H21" s="8" t="e">
-        <f xml:space="preserve"> Week3!G21 - Week10!G21</f>
+        <f xml:space="preserve"> Week3!G21 - Week11!G21</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J21" s="12"/>
@@ -3770,7 +4646,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H28" s="8" t="e">
-        <f xml:space="preserve"> Week3!G2 - Week10!G28</f>
+        <f xml:space="preserve"> Week3!G2 - Week11!G28</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J28" s="12"/>
@@ -3787,11 +4663,11 @@
       <c r="E29" s="12"/>
       <c r="F29" s="5"/>
       <c r="G29" s="8" t="e">
-        <f t="shared" ref="G29:G35" si="3">(ABS(E29 -F29)/MAX(ABS(E29),ABS(F29)) )* 100</f>
+        <f t="shared" ref="G29:G35" si="2">(ABS(E29 -F29)/MAX(ABS(E29),ABS(F29)) )* 100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H29" s="8" t="e">
-        <f xml:space="preserve"> Week3!G3 - Week10!G29</f>
+        <f xml:space="preserve"> Week3!G3 - Week11!G29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J29" s="12"/>
@@ -3807,11 +4683,11 @@
       <c r="D30" s="10"/>
       <c r="E30" s="12"/>
       <c r="G30" s="8" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H30" s="8" t="e">
-        <f xml:space="preserve"> Week3!G4 - Week10!G30</f>
+        <f xml:space="preserve"> Week3!G4 - Week11!G30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J30" s="12"/>
@@ -3828,11 +4704,11 @@
       <c r="E31" s="12"/>
       <c r="F31" s="5"/>
       <c r="G31" s="8" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H31" s="8" t="e">
-        <f xml:space="preserve"> Week3!G5 - Week10!G31</f>
+        <f xml:space="preserve"> Week3!G5 - Week11!G31</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J31" s="12"/>
@@ -3849,11 +4725,11 @@
       <c r="E32" s="12"/>
       <c r="F32" s="5"/>
       <c r="G32" s="8" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H32" s="8" t="e">
-        <f xml:space="preserve"> Week3!G6 - Week10!G32</f>
+        <f xml:space="preserve"> Week3!G6 - Week11!G32</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J32" s="12"/>
@@ -3865,27 +4741,19 @@
       <c r="B33">
         <v>6</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" s="12">
-        <v>-0.12430862230397099</v>
-      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="8">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="H33" s="8">
-        <f xml:space="preserve"> Week3!G7 - Week10!G33</f>
-        <v>-38.753477525597134</v>
-      </c>
-      <c r="J33" s="12">
-        <v>-0.22564673102918401</v>
-      </c>
+      <c r="G33" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="8" t="e">
+        <f xml:space="preserve"> Week3!G7 - Week11!G33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33" s="12"/>
     </row>
     <row r="34" spans="1:10" ht="18">
       <c r="A34">
@@ -3894,27 +4762,21 @@
       <c r="B34">
         <v>7</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>183</v>
-      </c>
+      <c r="C34" s="12"/>
       <c r="D34" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E34" s="12">
-        <v>1.88380795677045</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="E34" s="12"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="8">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="H34" s="8">
-        <f xml:space="preserve"> Week3!G8 - Week10!G34</f>
-        <v>-70.691643968564648</v>
-      </c>
-      <c r="J34" s="12">
-        <v>1.79243618860138</v>
-      </c>
+      <c r="G34" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="8" t="e">
+        <f xml:space="preserve"> Week3!G8 - Week11!G34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:10" ht="18">
       <c r="A35">
@@ -3923,27 +4785,19 @@
       <c r="B35">
         <v>8</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E35" s="12">
-        <v>9.9707717627203998</v>
-      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="8">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="H35" s="8">
-        <f xml:space="preserve"> Week3!G9 - Week10!G35</f>
-        <v>-97.559723769512345</v>
-      </c>
-      <c r="J35" s="12">
-        <v>10.051246412332</v>
-      </c>
+      <c r="G35" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="8" t="e">
+        <f xml:space="preserve"> Week3!G9 - Week11!G35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>